<commit_message>
Second version of IAV model without variable D and with some modifications.
</commit_message>
<xml_diff>
--- a/data_to_fit.xlsx
+++ b/data_to_fit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\MATLAB\immunity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\MATLAB\immunity-matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="57">
   <si>
     <t>CD45 cells (as % of all live cells)</t>
   </si>
@@ -186,51 +186,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Lung CD8 Tcell (as % of all live cells)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lung CD8 T_E cell (as % of all live cells)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZT23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZT11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t(ZT11)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t(ZT11)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t(ZT11)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Lung CD8_E (as % of CD45)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lung CD8 Tcell (as % of all live cells)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>day8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>day10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lung CD8 T_E cell (as % of all live cells)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZT23</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZT11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>day8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>day10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>t(ZT11)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>t(ZT11)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>t(ZT11)</t>
+    <t>Lung CD8 Tcell (as % of all live cells) without T_E</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -892,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84:C85"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2367,10 +2371,10 @@
         <v>40</v>
       </c>
       <c r="B70" s="31">
-        <v>10.548333333333334</v>
+        <v>22.666667</v>
       </c>
       <c r="C70" s="31">
-        <v>11.178000000000001</v>
+        <v>19.28</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2378,15 +2382,15 @@
         <v>41</v>
       </c>
       <c r="B71" s="31">
-        <v>17.466666666666665</v>
+        <v>30</v>
       </c>
       <c r="C71" s="31">
-        <v>14.975</v>
+        <v>28.774999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="31" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B73" s="31" t="s">
         <v>39</v>
@@ -2400,10 +2404,10 @@
         <v>42</v>
       </c>
       <c r="B74" s="31">
-        <v>1.9633333333333336</v>
+        <v>18.666666666666668</v>
       </c>
       <c r="C74" s="31">
-        <v>2.3199999999999998</v>
+        <v>15.68</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2411,15 +2415,15 @@
         <v>41</v>
       </c>
       <c r="B75" s="31">
-        <v>2.2783333333333329</v>
+        <v>25.241667</v>
       </c>
       <c r="C75" s="31">
-        <v>2.7424999999999997</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2432,71 +2436,116 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B79" s="31">
         <f>B70*B7*0.01</f>
-        <v>7.9956366666666669</v>
+        <v>17.181333586000001</v>
       </c>
       <c r="C79" s="31">
         <f>C70*E7*0.01</f>
-        <v>7.2433440000000004</v>
+        <v>12.493440000000001</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B80" s="31">
         <f>B71*B7*0.01</f>
-        <v>13.239733333333332</v>
+        <v>22.740000000000002</v>
       </c>
       <c r="C80" s="31">
         <f>C71*E7*0.01</f>
-        <v>9.7037999999999993</v>
+        <v>18.6462</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B83" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C83" s="31" t="s">
         <v>49</v>
-      </c>
-      <c r="C83" s="31" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B84" s="31">
         <f>B74*B7*0.01</f>
-        <v>1.4882066666666669</v>
+        <v>14.149333333333335</v>
       </c>
       <c r="C84" s="31">
         <f>C74*E7*0.01</f>
-        <v>1.5033599999999998</v>
+        <v>10.160639999999999</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B85" s="31">
         <f>B75*B7*0.01</f>
-        <v>1.7269766666666664</v>
+        <v>19.133183586000001</v>
       </c>
       <c r="C85" s="31">
         <f>C75*E7*0.01</f>
-        <v>1.7771399999999997</v>
+        <v>15.1632</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B88" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89" s="31">
+        <f>B79-B84</f>
+        <v>3.0320002526666663</v>
+      </c>
+      <c r="C89" s="31">
+        <f>C79-C84</f>
+        <v>2.3328000000000024</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B90" s="31">
+        <f>B80-B85</f>
+        <v>3.6068164140000007</v>
+      </c>
+      <c r="C90" s="31">
+        <f>C80-C85</f>
+        <v>3.4830000000000005</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
     <mergeCell ref="B51:D51"/>
     <mergeCell ref="E51:G51"/>
     <mergeCell ref="B26:D26"/>
@@ -2505,12 +2554,6 @@
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2523,7 +2566,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2679,7 +2722,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="31">
         <v>24</v>
@@ -2730,7 +2773,7 @@
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="39">
         <v>6</v>
@@ -2790,13 +2833,25 @@
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="39">
+        <v>54</v>
+      </c>
+      <c r="B20" s="31">
+        <v>24</v>
+      </c>
+      <c r="C20" s="31">
+        <v>48</v>
+      </c>
+      <c r="D20" s="31">
+        <v>96</v>
+      </c>
+      <c r="E20" s="31">
+        <v>144</v>
+      </c>
+      <c r="F20" s="39">
         <f>8*24</f>
         <v>192</v>
       </c>
-      <c r="C20" s="39">
+      <c r="G20" s="39">
         <f>10*24</f>
         <v>240</v>
       </c>
@@ -2806,10 +2861,22 @@
         <v>37</v>
       </c>
       <c r="B21" s="31">
-        <v>7.2433440000000004</v>
+        <v>0.05</v>
       </c>
       <c r="C21" s="31">
-        <v>9.7037999999999993</v>
+        <v>0.08</v>
+      </c>
+      <c r="D21" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="31">
+        <v>2.3328000000000002</v>
+      </c>
+      <c r="G21" s="31">
+        <v>3.4830000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2817,10 +2884,22 @@
         <v>38</v>
       </c>
       <c r="B22" s="31">
-        <v>1.5033599999999998</v>
+        <v>0.05</v>
       </c>
       <c r="C22" s="31">
-        <v>1.7771399999999997</v>
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="31">
+        <v>1</v>
+      </c>
+      <c r="F22" s="31">
+        <v>10.160639999999999</v>
+      </c>
+      <c r="G22" s="31">
+        <v>15.1632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fit of clock controlled IAV infection model.
</commit_message>
<xml_diff>
--- a/data_to_fit.xlsx
+++ b/data_to_fit.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="64">
   <si>
     <t>CD45 cells (as % of all live cells)</t>
   </si>
@@ -235,6 +236,34 @@
   </si>
   <si>
     <t>Lung CD8 Tcell (as % of all live cells) without T_E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZT23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZT11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_E</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -899,7 +928,7 @@
   <dimension ref="A1:N90"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2540,12 +2569,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
     <mergeCell ref="B51:D51"/>
     <mergeCell ref="E51:G51"/>
     <mergeCell ref="B26:D26"/>
@@ -2554,6 +2577,12 @@
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2565,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2689,11 +2718,23 @@
       <c r="A8" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="31">
+        <v>24</v>
+      </c>
+      <c r="C8" s="31">
+        <v>48</v>
+      </c>
+      <c r="D8" s="31">
+        <v>96</v>
+      </c>
+      <c r="E8" s="31">
+        <v>144</v>
+      </c>
+      <c r="F8" s="39">
         <f>8*24</f>
         <v>192</v>
       </c>
-      <c r="C8" s="39">
+      <c r="G8" s="39">
         <f>10*24</f>
         <v>240</v>
       </c>
@@ -2703,10 +2744,22 @@
         <v>37</v>
       </c>
       <c r="B9" s="31">
-        <v>7.9956366666666696</v>
+        <v>0.05</v>
       </c>
       <c r="C9" s="31">
-        <v>13.239733333333332</v>
+        <v>0.08</v>
+      </c>
+      <c r="D9" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="31">
+        <v>3.0320002526666663</v>
+      </c>
+      <c r="G9" s="31">
+        <v>3.6068164140000007</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2714,10 +2767,22 @@
         <v>38</v>
       </c>
       <c r="B10" s="31">
-        <v>1.4882066666666669</v>
+        <v>0.05</v>
       </c>
       <c r="C10" s="31">
-        <v>1.7269766666666664</v>
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="31">
+        <v>1</v>
+      </c>
+      <c r="F10" s="31">
+        <v>14.149333333333335</v>
+      </c>
+      <c r="G10" s="31">
+        <v>19.133183586000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2907,4 +2972,356 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="31">
+        <v>24</v>
+      </c>
+      <c r="C1" s="31">
+        <v>48</v>
+      </c>
+      <c r="D1" s="31">
+        <v>96</v>
+      </c>
+      <c r="E1" s="31">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="31">
+        <v>13.02786</v>
+      </c>
+      <c r="C2" s="31">
+        <v>17.766539999999999</v>
+      </c>
+      <c r="D2" s="31">
+        <v>23.985200000000003</v>
+      </c>
+      <c r="E2" s="31">
+        <v>40.158839999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="31">
+        <v>19.958400000000001</v>
+      </c>
+      <c r="C3" s="31">
+        <v>28.712300000000003</v>
+      </c>
+      <c r="D3" s="31">
+        <v>36.297600000000003</v>
+      </c>
+      <c r="E3" s="31">
+        <v>33.307200000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="31">
+        <v>24</v>
+      </c>
+      <c r="C5" s="31">
+        <v>48</v>
+      </c>
+      <c r="D5" s="31">
+        <v>96</v>
+      </c>
+      <c r="E5" s="31">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="31">
+        <v>5.2554000000000007</v>
+      </c>
+      <c r="C6" s="31">
+        <v>6.7003199999999996</v>
+      </c>
+      <c r="D6" s="31">
+        <v>7.9910000000000005</v>
+      </c>
+      <c r="E6" s="31">
+        <v>9.3234000000000012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="31">
+        <v>6.2207999999999997</v>
+      </c>
+      <c r="C7" s="31">
+        <v>4.8201499999999999</v>
+      </c>
+      <c r="D7" s="31">
+        <v>7.1440000000000001</v>
+      </c>
+      <c r="E7" s="31">
+        <v>7.7759999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="39">
+        <v>6</v>
+      </c>
+      <c r="C9" s="39">
+        <v>12</v>
+      </c>
+      <c r="D9" s="31">
+        <v>24</v>
+      </c>
+      <c r="E9" s="31">
+        <v>48</v>
+      </c>
+      <c r="F9" s="31">
+        <v>96</v>
+      </c>
+      <c r="G9" s="31">
+        <v>144</v>
+      </c>
+      <c r="H9" s="39">
+        <f>8*24</f>
+        <v>192</v>
+      </c>
+      <c r="I9" s="39">
+        <f>10*24</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="31">
+        <v>0</v>
+      </c>
+      <c r="C10" s="31">
+        <v>1.65</v>
+      </c>
+      <c r="D10" s="31">
+        <v>4.6000000000000005</v>
+      </c>
+      <c r="E10" s="31">
+        <v>4.7250000000000005</v>
+      </c>
+      <c r="F10" s="31">
+        <v>5.55</v>
+      </c>
+      <c r="G10" s="31">
+        <v>5.1000000000000005</v>
+      </c>
+      <c r="H10" s="31">
+        <v>3.4249999999999998</v>
+      </c>
+      <c r="I10" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="31">
+        <v>0</v>
+      </c>
+      <c r="C11" s="31">
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="D11" s="31">
+        <v>5.1749999999999998</v>
+      </c>
+      <c r="E11" s="31">
+        <v>4.7750000000000004</v>
+      </c>
+      <c r="F11" s="31">
+        <v>5.6749999999999998</v>
+      </c>
+      <c r="G11" s="31">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="H11" s="31">
+        <v>4.5</v>
+      </c>
+      <c r="I11" s="31">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="31">
+        <v>24</v>
+      </c>
+      <c r="C13" s="31">
+        <v>48</v>
+      </c>
+      <c r="D13" s="31">
+        <v>96</v>
+      </c>
+      <c r="E13" s="31">
+        <v>144</v>
+      </c>
+      <c r="F13" s="39">
+        <f>8*24</f>
+        <v>192</v>
+      </c>
+      <c r="G13" s="39">
+        <f>10*24</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="C14" s="31">
+        <v>0.08</v>
+      </c>
+      <c r="D14" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="31">
+        <v>3.0320002526666663</v>
+      </c>
+      <c r="G14" s="31">
+        <v>3.6068164140000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="C15" s="31">
+        <v>0.08</v>
+      </c>
+      <c r="D15" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="31">
+        <v>2.3328000000000002</v>
+      </c>
+      <c r="G15" s="31">
+        <v>3.4830000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="31">
+        <v>24</v>
+      </c>
+      <c r="C17" s="31">
+        <v>48</v>
+      </c>
+      <c r="D17" s="31">
+        <v>96</v>
+      </c>
+      <c r="E17" s="31">
+        <v>144</v>
+      </c>
+      <c r="F17" s="39">
+        <f>8*24</f>
+        <v>192</v>
+      </c>
+      <c r="G17" s="39">
+        <f>10*24</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="31">
+        <v>1</v>
+      </c>
+      <c r="F18" s="31">
+        <v>14.149333333333335</v>
+      </c>
+      <c r="G18" s="31">
+        <v>19.133183586000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="31">
+        <v>1</v>
+      </c>
+      <c r="F19" s="31">
+        <v>10.160639999999999</v>
+      </c>
+      <c r="G19" s="31">
+        <v>15.1632</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>